<commit_message>
[FIX] Carga no lectiva
</commit_message>
<xml_diff>
--- a/EXCEL_TRABAJADO/2023-2.xlsx
+++ b/EXCEL_TRABAJADO/2023-2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gians\Desktop\dev\UNDC_AUTOMATIZACION\EXCEL_TRABAJADO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1167FEF-01AA-4B94-9A02-EBE9D6A0E015}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC3D2761-B58E-44F1-A465-B4E727A54AD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="768" uniqueCount="311">
   <si>
     <t>N°</t>
   </si>
@@ -940,6 +940,21 @@
   </si>
   <si>
     <t>https://aula.undc.edu.pe/course/view.php?id=355</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>AG56 - 611 - EDAFOLOGIA - 3643</t>
+  </si>
+  <si>
+    <t>NOCHE</t>
+  </si>
+  <si>
+    <t>https://aula.undc.edu.pe/course/view.php?id=391</t>
+  </si>
+  <si>
+    <t>https://chat.whatsapp.com/IhQbHsVHmumJCBSYFiiM0L</t>
   </si>
 </sst>
 </file>
@@ -1433,11 +1448,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="A1:AE70"/>
+  <dimension ref="A1:AE71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T69" sqref="T69"/>
+      <selection pane="bottomLeft" activeCell="AB71" sqref="AB71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5938,7 +5953,7 @@
         <v>303</v>
       </c>
       <c r="V68" t="str">
-        <f t="shared" ref="V68:V70" si="11">MID(U68,45,4)</f>
+        <f t="shared" ref="V68:V71" si="11">MID(U68,45,4)</f>
         <v>354</v>
       </c>
       <c r="W68" t="str">
@@ -6066,7 +6081,7 @@
       <c r="T70" t="s">
         <v>236</v>
       </c>
-      <c r="U70" t="s">
+      <c r="U70" s="8" t="s">
         <v>305</v>
       </c>
       <c r="V70" t="str">
@@ -6098,10 +6113,80 @@
         <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/Fhnw0QvZFhGKOPV27MUfye' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
       </c>
     </row>
+    <row r="71" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>32</v>
+      </c>
+      <c r="B71" t="s">
+        <v>17</v>
+      </c>
+      <c r="C71" t="s">
+        <v>306</v>
+      </c>
+      <c r="D71" t="s">
+        <v>307</v>
+      </c>
+      <c r="E71" t="s">
+        <v>57</v>
+      </c>
+      <c r="F71" t="s">
+        <v>308</v>
+      </c>
+      <c r="G71" t="s">
+        <v>20</v>
+      </c>
+      <c r="H71">
+        <v>2</v>
+      </c>
+      <c r="I71" t="s">
+        <v>75</v>
+      </c>
+      <c r="S71" t="s">
+        <v>310</v>
+      </c>
+      <c r="T71" t="s">
+        <v>236</v>
+      </c>
+      <c r="U71" s="8" t="s">
+        <v>309</v>
+      </c>
+      <c r="V71" t="str">
+        <f t="shared" si="11"/>
+        <v>391</v>
+      </c>
+      <c r="W71" t="str">
+        <f t="shared" ref="W71" si="16">MID(D71,1,10)</f>
+        <v>AG56 - 611</v>
+      </c>
+      <c r="X71" t="str">
+        <f t="shared" ref="X71" si="17">TRIM(MID(D71,14,222))</f>
+        <v>EDAFOLOGIA - 3643</v>
+      </c>
+      <c r="Y71" t="str">
+        <f t="shared" ref="Y71" si="18">TRIM(CONCATENATE("AGRONOMIA ",E71,"-",F71,"-",G71," ",LEFT(X71,LEN(X71)-7)))</f>
+        <v>AGRONOMIA V-NOCHE-A EDAFOLOGIA</v>
+      </c>
+      <c r="Z71" t="str">
+        <f t="shared" ref="Z71" si="19">CONCATENATE(B71,"_",E71,"-",IF(F71="MANANA","M",IF(F71="MAÑANA","M",IF(F71="TARDE","T",IF(F71="NOCHE","N","NO EXISITE")))),"-",G71," ",X71)</f>
+        <v>AG_V-N-A EDAFOLOGIA - 3643</v>
+      </c>
+      <c r="AA71" t="str">
+        <f t="shared" ref="AA71" si="20">TRIM(MID(Z71,1,25))</f>
+        <v>AG_V-N-A EDAFOLOGIA - 364</v>
+      </c>
+      <c r="AB71" t="str">
+        <f>CONCATENATE("&lt;p&gt;&lt;a href='",S71,"' target='_blank'&gt;&lt;img src='",items!$B$1,"' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;")</f>
+        <v>&lt;p&gt;&lt;a href='https://chat.whatsapp.com/IhQbHsVHmumJCBSYFiiM0L' target='_blank'&gt;&lt;img src='https://firebasestorage.googleapis.com/v0/b/backup-a2b5c.appspot.com/o/linkwhatsapp.png?alt=media&amp;token=531801e8-d490-42f7-b704-64c0f96eb8c5' alt='' width='291' height='42' role='presentation' class='img-responsive atto_image_button_text-bottom'&gt;&lt;/a&gt;&lt;br&gt;&lt;/p&gt;</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="U70" r:id="rId1" xr:uid="{40E0ACC9-A317-4F17-AE70-75293C498E70}"/>
+    <hyperlink ref="U71" r:id="rId2" xr:uid="{1E811D99-E623-429D-B660-C5E01AC03687}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -6368,7 +6453,7 @@
       </c>
       <c r="B8">
         <f>COUNTIFS(Sheet!E:E,items!A8)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -6419,7 +6504,7 @@
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B14">
         <f>SUM(B4:B13)</f>
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>